<commit_message>
new user method added
</commit_message>
<xml_diff>
--- a/src/main/java/data/data.xlsx
+++ b/src/main/java/data/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>title</t>
   </si>
@@ -66,23 +66,47 @@
     <t>Ebay</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>falcoconstantine</t>
-  </si>
-  <si>
     <t>A6milionierius</t>
+  </si>
+  <si>
+    <t>mailtofalco@gmail.com</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Falco</t>
+  </si>
+  <si>
+    <t>Constantine</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +114,14 @@
       <family val="2"/>
       <charset val="186"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
     </font>
   </fonts>
   <fills count="4">
@@ -121,15 +153,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -434,35 +477,103 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" s="4" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1983</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1"/>
+    <row r="4" spans="1:11" s="4" customFormat="1"/>
+    <row r="5" spans="1:11" s="4" customFormat="1"/>
+    <row r="6" spans="1:11" s="4" customFormat="1"/>
+    <row r="7" spans="1:11" s="4" customFormat="1"/>
+    <row r="8" spans="1:11" s="4" customFormat="1"/>
+    <row r="9" spans="1:11" s="4" customFormat="1"/>
+    <row r="10" spans="1:11" s="4" customFormat="1"/>
+    <row r="11" spans="1:11" s="4" customFormat="1"/>
+    <row r="12" spans="1:11" s="4" customFormat="1"/>
+    <row r="13" spans="1:11" s="4" customFormat="1"/>
+    <row r="14" spans="1:11" s="4" customFormat="1"/>
+    <row r="15" spans="1:11" s="4" customFormat="1"/>
+    <row r="16" spans="1:11" s="4" customFormat="1"/>
+    <row r="17" s="4" customFormat="1"/>
+    <row r="18" s="4" customFormat="1"/>
+    <row r="19" s="4" customFormat="1"/>
+    <row r="20" s="4" customFormat="1"/>
+    <row r="21" s="4" customFormat="1"/>
+    <row r="22" s="4" customFormat="1"/>
+    <row r="23" s="4" customFormat="1"/>
+    <row r="24" s="4" customFormat="1"/>
+    <row r="25" s="4" customFormat="1"/>
+    <row r="26" s="4" customFormat="1"/>
+    <row r="27" s="4" customFormat="1"/>
+    <row r="28" s="4" customFormat="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
pre-test method added for all framework activity validation
</commit_message>
<xml_diff>
--- a/src/main/java/data/data.xlsx
+++ b/src/main/java/data/data.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15570" windowHeight="4440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="15945" windowHeight="7095"/>
   </bookViews>
   <sheets>
-    <sheet name="contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="main_menu_smoke" sheetId="1" r:id="rId1"/>
     <sheet name="users" sheetId="2" r:id="rId2"/>
     <sheet name="deals" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:J22"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>title</t>
   </si>
@@ -100,6 +101,33 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>3 tab</t>
+  </si>
+  <si>
+    <t>4 tab</t>
+  </si>
+  <si>
+    <t>5 tab</t>
+  </si>
+  <si>
+    <t>6 tab</t>
+  </si>
+  <si>
+    <t>7 tab</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Euro</t>
+  </si>
+  <si>
+    <t>currency</t>
   </si>
 </sst>
 </file>
@@ -124,7 +152,7 @@
       <charset val="186"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +168,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,7 +194,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -170,6 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -465,12 +500,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -479,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>